<commit_message>
Time Sheet update for week 3
</commit_message>
<xml_diff>
--- a/Time Sheet.xlsx
+++ b/Time Sheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="28800" windowHeight="16120"/>
   </bookViews>
   <sheets>
     <sheet name="Time Sheet" sheetId="1" r:id="rId1"/>
@@ -680,8 +680,8 @@
   </sheetPr>
   <dimension ref="B1:I34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -751,15 +751,14 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>79</v>
+        <v>117.5</v>
       </c>
       <c r="D6" s="3">
-        <f>IFERROR(IF(C6&lt;=WorkweekHours,C6,WorkweekHours),"")</f>
-        <v>35</v>
+        <v>175</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-D6, "")</f>
-        <v>44</v>
+        <v>-57.5</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -1006,70 +1005,110 @@
       <c r="B18" s="13">
         <v>43661</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
+      <c r="C18" s="14">
+        <v>0.375</v>
+      </c>
+      <c r="D18" s="14">
+        <v>0.5625</v>
+      </c>
+      <c r="E18" s="14">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="F18" s="14">
+        <v>0.75</v>
+      </c>
       <c r="G18" s="15">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="13">
         <v>43662</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
+      <c r="C19" s="14">
+        <v>0.375</v>
+      </c>
+      <c r="D19" s="14">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E19" s="14">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F19" s="14">
+        <v>0.72916666666666663</v>
+      </c>
       <c r="G19" s="15">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>7.4999999999999973</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="13">
         <v>43663</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
+      <c r="C20" s="14">
+        <v>0.375</v>
+      </c>
+      <c r="D20" s="14">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E20" s="14">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F20" s="14">
+        <v>0.72916666666666663</v>
+      </c>
       <c r="G20" s="15">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>7.4999999999999973</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="13">
         <v>43664</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
+      <c r="C21" s="14">
+        <v>0.375</v>
+      </c>
+      <c r="D21" s="14">
+        <v>0.5625</v>
+      </c>
+      <c r="E21" s="14">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="F21" s="14">
+        <v>0.75</v>
+      </c>
       <c r="G21" s="15">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="2:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="22">
         <v>43665</v>
       </c>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
+      <c r="C22" s="23">
+        <v>0.375</v>
+      </c>
+      <c r="D22" s="23">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E22" s="23">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F22" s="23">
+        <v>0.72916666666666663</v>
+      </c>
       <c r="G22" s="24">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>7.4999999999999973</v>
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="21">
         <f>SUM(G18:G22)</f>
-        <v>0</v>
+        <v>38.499999999999993</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1223,7 +1262,7 @@
       </c>
       <c r="I33" s="16">
         <f>SUM(I12,I17,I22,I27,I32)</f>
-        <v>79</v>
+        <v>117.5</v>
       </c>
     </row>
     <row r="34" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1237,7 +1276,7 @@
       </c>
       <c r="I34">
         <f>I33/5</f>
-        <v>15.8</v>
+        <v>23.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Working Protocol and Time Sheet Lotteritsch
</commit_message>
<xml_diff>
--- a/Time Sheet.xlsx
+++ b/Time Sheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="28800" windowHeight="16120"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="28800" windowHeight="16120"/>
   </bookViews>
   <sheets>
     <sheet name="Time Sheet" sheetId="1" r:id="rId1"/>
@@ -681,7 +681,7 @@
   <dimension ref="B1:I34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -751,14 +751,14 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>117.5</v>
+        <v>153.5</v>
       </c>
       <c r="D6" s="3">
         <v>175</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-D6, "")</f>
-        <v>-57.5</v>
+        <v>-21.5</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -1115,70 +1115,110 @@
       <c r="B23" s="13">
         <v>43668</v>
       </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
+      <c r="C23" s="14">
+        <v>0.375</v>
+      </c>
+      <c r="D23" s="14">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E23" s="14">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F23" s="14">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="G23" s="15">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>6.9999999999999991</v>
       </c>
     </row>
     <row r="24" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="13">
         <v>43669</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
+      <c r="C24" s="14">
+        <v>0.375</v>
+      </c>
+      <c r="D24" s="14">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E24" s="14">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F24" s="14">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="G24" s="15">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>6.9999999999999991</v>
       </c>
     </row>
     <row r="25" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="13">
         <v>43670</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
+      <c r="C25" s="14">
+        <v>0.375</v>
+      </c>
+      <c r="D25" s="14">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E25" s="14">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F25" s="14">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="G25" s="15">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>6.9999999999999991</v>
       </c>
     </row>
     <row r="26" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="13">
         <v>43671</v>
       </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
+      <c r="C26" s="14">
+        <v>0.375</v>
+      </c>
+      <c r="D26" s="14">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E26" s="14">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F26" s="14">
+        <v>0.72916666666666663</v>
+      </c>
       <c r="G26" s="15">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>7.4999999999999973</v>
       </c>
     </row>
     <row r="27" spans="2:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="22">
         <v>43672</v>
       </c>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
+      <c r="C27" s="23">
+        <v>0.375</v>
+      </c>
+      <c r="D27" s="23">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E27" s="23">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F27" s="23">
+        <v>0.72916666666666663</v>
+      </c>
       <c r="G27" s="24">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>7.4999999999999973</v>
       </c>
       <c r="H27" s="20"/>
       <c r="I27" s="21">
         <f>SUM(G23:G27)</f>
-        <v>0</v>
+        <v>35.999999999999993</v>
       </c>
     </row>
     <row r="28" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1262,7 +1302,7 @@
       </c>
       <c r="I33" s="16">
         <f>SUM(I12,I17,I22,I27,I32)</f>
-        <v>117.5</v>
+        <v>153.5</v>
       </c>
     </row>
     <row r="34" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1276,7 +1316,7 @@
       </c>
       <c r="I34">
         <f>I33/5</f>
-        <v>23.5</v>
+        <v>30.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>